<commit_message>
commit 10/8/2022 Registration Password Module
</commit_message>
<xml_diff>
--- a/Advanced_Selenium_Test_Automation_Framework-master/src/test/resources/testData/TaskCreationTestData.xlsx
+++ b/Advanced_Selenium_Test_Automation_Framework-master/src/test/resources/testData/TaskCreationTestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advanced_Selenium_Test_Automation_Framework-master\Advanced_Selenium_Test_Automation_Framework-master\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4577CF7D-DBDC-439A-B9CD-6DCED9396BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD26248F-3CB1-4D39-9F07-46FEBF302B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskCreationData" sheetId="1" r:id="rId1"/>
     <sheet name="validLogin" sheetId="2" r:id="rId2"/>
     <sheet name="invalidLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="registration" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Sr No</t>
   </si>
@@ -147,6 +148,27 @@
   </si>
   <si>
     <t>User123</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>Mayank</t>
+  </si>
+  <si>
+    <t>Upendra</t>
+  </si>
+  <si>
+    <t>Mishra</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
   </si>
 </sst>
 </file>
@@ -700,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFEA53E-5F55-4A90-B690-C1CBC93B39DB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,4 +789,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8489DCB3-BD85-43AA-A4F1-631114C33A41}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1C38B1EC-822F-4EC6-9374-747C178E6C8A}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{9BCA5B6D-8A05-469D-B0FB-2DC68F132570}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>